<commit_message>
Added Taxable Services dropdown list on bulk invoice import UI.
</commit_message>
<xml_diff>
--- a/rev/bulkInvoiceImport/usr/Template.xlsx
+++ b/rev/bulkInvoiceImport/usr/Template.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Quantity</t>
   </si>
@@ -78,6 +78,9 @@
   </si>
   <si>
     <t>InvoiceByHouseCode</t>
+  </si>
+  <si>
+    <t>TaxableService</t>
   </si>
 </sst>
 </file>
@@ -957,10 +960,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T2"/>
+  <dimension ref="A1:U2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="T1" sqref="T1"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="U1" sqref="U1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -984,9 +987,10 @@
     <col min="18" max="18" width="9.140625" style="6"/>
     <col min="19" max="19" width="10.42578125" customWidth="1"/>
     <col min="20" max="20" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="3" customFormat="1">
+    <row r="1" spans="1:21" s="3" customFormat="1">
       <c r="A1" s="8" t="s">
         <v>3</v>
       </c>
@@ -1047,8 +1051,11 @@
       <c r="T1" s="3" t="s">
         <v>19</v>
       </c>
+      <c r="U1" s="3" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:21">
       <c r="H2" s="13"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Set the Invoice Due Date based on Payment Terms Code due days [TF00373].
</commit_message>
<xml_diff>
--- a/rev/bulkInvoiceImport/usr/Template.xlsx
+++ b/rev/bulkInvoiceImport/usr/Template.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Sequence</t>
   </si>
@@ -70,9 +70,6 @@
   </si>
   <si>
     <t>Invoice Date</t>
-  </si>
-  <si>
-    <t>Due Date</t>
   </si>
   <si>
     <t>Service Start Date</t>
@@ -431,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V1"/>
+  <dimension ref="A1:U1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <selection activeCell="J1" sqref="J1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -447,21 +444,21 @@
     <col min="6" max="6" width="16.42578125" customWidth="1"/>
     <col min="7" max="7" width="15.140625" customWidth="1"/>
     <col min="8" max="8" width="13.85546875" customWidth="1"/>
-    <col min="9" max="10" width="15.140625" customWidth="1"/>
-    <col min="11" max="11" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.85546875" customWidth="1"/>
-    <col min="14" max="14" width="35.28515625" customWidth="1"/>
-    <col min="15" max="15" width="10.5703125" customWidth="1"/>
-    <col min="17" max="17" width="14" customWidth="1"/>
-    <col min="18" max="18" width="14.140625" customWidth="1"/>
-    <col min="19" max="19" width="11.7109375" customWidth="1"/>
-    <col min="20" max="20" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="29.7109375" customWidth="1"/>
-    <col min="22" max="22" width="18.7109375" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.85546875" customWidth="1"/>
+    <col min="13" max="13" width="35.28515625" customWidth="1"/>
+    <col min="14" max="14" width="10.5703125" customWidth="1"/>
+    <col min="16" max="16" width="14" customWidth="1"/>
+    <col min="17" max="17" width="14.140625" customWidth="1"/>
+    <col min="18" max="18" width="11.7109375" customWidth="1"/>
+    <col min="19" max="19" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="29.7109375" customWidth="1"/>
+    <col min="21" max="21" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -499,33 +496,30 @@
         <v>20</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="V1" s="1" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>